<commit_message>
creating individual column for exemption types
</commit_message>
<xml_diff>
--- a/Ada County (003)TestOutput.xlsx
+++ b/Ada County (003)TestOutput.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:P115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,36 @@
           <t>Net Value</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Site Improvements</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Remediated Land</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Pollution</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>New Capital Investments</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Casualty</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -524,6 +554,12 @@
           <t>70133800.0</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -562,6 +598,12 @@
           <t>1253400.0</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -600,6 +642,12 @@
           <t>518200.0</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -640,6 +688,12 @@
           <t>8034500.0</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -678,6 +732,12 @@
           <t>25600.0</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -718,6 +778,12 @@
           <t>440720113.0</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -758,6 +824,12 @@
           <t>536500.0</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -798,6 +870,12 @@
           <t>25038600.0</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -832,6 +910,12 @@
           <t>25575100.0</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -872,6 +956,12 @@
           <t>44050400.0</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -912,6 +1002,12 @@
           <t>430281531.0</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -952,6 +1048,12 @@
           <t>474331931.0</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -992,6 +1094,12 @@
           <t>11859100.0</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1032,6 +1140,12 @@
           <t>47423300.0</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1066,6 +1180,12 @@
           <t>59282400.0</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1106,6 +1226,12 @@
           <t>3282900.0</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1146,6 +1272,12 @@
           <t>15631000.0</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1182,6 +1314,12 @@
           <t>18913900.0</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1222,6 +1360,12 @@
           <t>154447400.0</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1252,6 +1396,16 @@
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>31356437.0 Site Improvements</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1292,6 +1446,12 @@
           <t>3885631079.0</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1330,6 +1490,12 @@
           <t>4040078479.0</t>
         </is>
       </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1370,6 +1536,12 @@
           <t>12733600.0</t>
         </is>
       </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1410,6 +1582,12 @@
           <t>23165000.0</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1444,6 +1622,12 @@
           <t>35898600.0</t>
         </is>
       </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1484,6 +1668,12 @@
           <t>8169200.0</t>
         </is>
       </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1514,6 +1704,16 @@
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>206400.0 Site Improvements</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1554,6 +1754,12 @@
           <t>10112300.0</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1588,6 +1794,12 @@
           <t>18281500.0</t>
         </is>
       </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1628,6 +1840,12 @@
           <t>361150200.0</t>
         </is>
       </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1658,6 +1876,16 @@
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>3368554.0 Site Improvements</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1698,6 +1926,12 @@
           <t>66441500.0</t>
         </is>
       </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1734,6 +1968,12 @@
           <t>427591700.0</t>
         </is>
       </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1772,6 +2012,12 @@
           <t>300.0</t>
         </is>
       </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1812,6 +2058,12 @@
           <t>1063602826.0</t>
         </is>
       </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1842,6 +2094,16 @@
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>195794146.0 Site Improvements</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1882,6 +2144,12 @@
           <t>27249993342.0</t>
         </is>
       </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1922,6 +2190,12 @@
           <t>28313596168.0</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1962,6 +2236,12 @@
           <t>957797200.0</t>
         </is>
       </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1992,6 +2272,16 @@
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>64400.0 Remediated Land</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2022,6 +2312,16 @@
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>37149054.0 Site Improvements</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2062,6 +2362,12 @@
           <t>4814605967.0</t>
         </is>
       </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2102,6 +2408,12 @@
           <t>5772403167.0</t>
         </is>
       </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2142,6 +2454,12 @@
           <t>190451500.0</t>
         </is>
       </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2182,6 +2500,12 @@
           <t>501807000.0</t>
         </is>
       </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2218,6 +2542,12 @@
           <t>692258500.0</t>
         </is>
       </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2258,6 +2588,12 @@
           <t>1237200.0</t>
         </is>
       </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2298,6 +2634,12 @@
           <t>869055034.0</t>
         </is>
       </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2334,6 +2676,12 @@
           <t>775093700.0</t>
         </is>
       </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2368,6 +2716,12 @@
           <t>201850.0</t>
         </is>
       </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2404,6 +2758,12 @@
           <t>536565877.0</t>
         </is>
       </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2440,6 +2800,12 @@
           <t>64542100.0</t>
         </is>
       </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2474,6 +2840,12 @@
           <t>25058800.0</t>
         </is>
       </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2514,6 +2886,12 @@
           <t>333407674.0</t>
         </is>
       </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2548,6 +2926,12 @@
           <t>75620900.0</t>
         </is>
       </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2582,6 +2966,12 @@
           <t>150955300.0</t>
         </is>
       </c>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2616,6 +3006,12 @@
           <t>4213931851.0</t>
         </is>
       </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2650,6 +3046,12 @@
           <t>43648300.0</t>
         </is>
       </c>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2684,6 +3086,12 @@
           <t>28652300.0</t>
         </is>
       </c>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2720,6 +3128,12 @@
           <t>25414500.0</t>
         </is>
       </c>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2760,6 +3174,12 @@
           <t>30611268025.0</t>
         </is>
       </c>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2790,6 +3210,16 @@
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>83422.0 Pollution</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2830,6 +3260,12 @@
           <t>13632996557.0</t>
         </is>
       </c>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2860,6 +3296,16 @@
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>309744.0 Pollution</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2890,6 +3336,16 @@
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>403434500.0 New Capital Investments</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2920,6 +3376,12 @@
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2956,6 +3418,12 @@
           <t>1779111300.0</t>
         </is>
       </c>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2996,6 +3464,12 @@
           <t>45782000.0</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3036,6 +3510,12 @@
           <t>35959252.0</t>
         </is>
       </c>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -3076,6 +3556,12 @@
           <t>86802259.0</t>
         </is>
       </c>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -3110,6 +3596,12 @@
           <t>15583550.0</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -3146,6 +3638,12 @@
           <t>110009400.0</t>
         </is>
       </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -3180,6 +3678,12 @@
           <t>1424500.0</t>
         </is>
       </c>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
@@ -3196,6 +3700,12 @@
         </is>
       </c>
       <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr"/>
@@ -3212,6 +3722,12 @@
         </is>
       </c>
       <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr"/>
@@ -3228,6 +3744,16 @@
         </is>
       </c>
       <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>-119000.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -3264,6 +3790,12 @@
           <t>836803200.0</t>
         </is>
       </c>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
@@ -3280,6 +3812,12 @@
         </is>
       </c>
       <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
@@ -3296,6 +3834,12 @@
         </is>
       </c>
       <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr"/>
@@ -3312,6 +3856,16 @@
         </is>
       </c>
       <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>-35644700.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -3352,6 +3906,12 @@
           <t>156717702.0</t>
         </is>
       </c>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -3382,6 +3942,16 @@
         </is>
       </c>
       <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>35373321.0 Pollution</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -3412,6 +3982,12 @@
         </is>
       </c>
       <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3442,6 +4018,16 @@
         </is>
       </c>
       <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>1257049000.0 New Capital Investments</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3478,6 +4064,12 @@
           <t>348723700.0</t>
         </is>
       </c>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -3494,6 +4086,12 @@
         </is>
       </c>
       <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr"/>
@@ -3510,6 +4108,12 @@
         </is>
       </c>
       <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -3526,6 +4130,16 @@
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>-485300.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3562,6 +4176,12 @@
           <t>25608000.0</t>
         </is>
       </c>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -3578,6 +4198,12 @@
         </is>
       </c>
       <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr"/>
@@ -3594,6 +4220,12 @@
         </is>
       </c>
       <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -3610,6 +4242,16 @@
         </is>
       </c>
       <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>-496400.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -3646,6 +4288,12 @@
           <t>7987000.0</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -3662,6 +4310,12 @@
         </is>
       </c>
       <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -3678,6 +4332,12 @@
         </is>
       </c>
       <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
@@ -3694,6 +4354,16 @@
         </is>
       </c>
       <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>-179800.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
@@ -3710,6 +4380,12 @@
         </is>
       </c>
       <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
@@ -3726,6 +4402,16 @@
         </is>
       </c>
       <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>64400.0 Remediated Land</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
@@ -3742,6 +4428,12 @@
         </is>
       </c>
       <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr"/>
@@ -3758,6 +4450,16 @@
         </is>
       </c>
       <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>35766487.0 Pollution</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr"/>
@@ -3774,6 +4476,12 @@
         </is>
       </c>
       <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
@@ -3790,6 +4498,16 @@
         </is>
       </c>
       <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> New Capital Investments</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr"/>
@@ -3806,6 +4524,16 @@
         </is>
       </c>
       <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Casualty</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr"/>
@@ -3822,6 +4550,12 @@
         </is>
       </c>
       <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr"/>
@@ -3838,6 +4572,12 @@
         </is>
       </c>
       <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr"/>
@@ -3854,6 +4594,12 @@
         </is>
       </c>
       <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr"/>
@@ -3870,6 +4616,12 @@
         </is>
       </c>
       <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr"/>
@@ -3886,6 +4638,12 @@
         </is>
       </c>
       <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr"/>
@@ -3902,6 +4660,12 @@
         </is>
       </c>
       <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr"/>
@@ -3918,6 +4682,12 @@
         </is>
       </c>
       <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr"/>
@@ -3934,6 +4704,12 @@
         </is>
       </c>
       <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr"/>
@@ -3950,6 +4726,16 @@
         </is>
       </c>
       <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>-36925200.0 PP Increment Exemption</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
@@ -3990,6 +4776,12 @@
           <t>95237059189.0</t>
         </is>
       </c>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr"/>
@@ -4006,6 +4798,12 @@
         </is>
       </c>
       <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>